<commit_message>
modified format0 method slightly to take R1 P1 and R1 P1 (1)
</commit_message>
<xml_diff>
--- a/maer_auto.xlsx
+++ b/maer_auto.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK26"/>
+  <dimension ref="A1:DI39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,275 +396,525 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>prt_1_vas.response_raw_i1650</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i1650</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i1650</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i1650</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>prt_order_i1650</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i1721</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i1721</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i1721</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i1721</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>prt_order_i1721</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
           <t>prt_1_vas.response_raw_i2057</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i2057</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i2057</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i2057</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>prt_order_i2057</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i2205</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i2205</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i2205</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i2205</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>prt_order_i2205</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i2276</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i2276</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i2276</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i2276</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>prt_order_i2276</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i2389</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i2389</t>
+        </is>
+      </c>
+      <c r="AJ1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i2389</t>
+        </is>
+      </c>
+      <c r="AK1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i2389</t>
+        </is>
+      </c>
+      <c r="AL1" t="inlineStr">
+        <is>
+          <t>prt_order_i2389</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i2393</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i2393</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i2393</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i2393</t>
+        </is>
+      </c>
+      <c r="AQ1" t="inlineStr">
+        <is>
+          <t>prt_order_i2393</t>
+        </is>
+      </c>
+      <c r="AR1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i2512</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="AS1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i2512</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="AT1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i2512</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="AU1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i2512</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="AV1" t="inlineStr">
         <is>
           <t>prt_order_i2512</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="AW1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i2745</t>
+        </is>
+      </c>
+      <c r="AX1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i2745</t>
+        </is>
+      </c>
+      <c r="AY1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i2745</t>
+        </is>
+      </c>
+      <c r="AZ1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i2745</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>prt_order_i2745</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i2750</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="BC1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i2750</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="BD1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i2750</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="BE1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i2750</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="BF1" t="inlineStr">
         <is>
           <t>prt_order_i2750</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="BG1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i2840</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="BH1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i2840</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="BI1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i2840</t>
         </is>
       </c>
-      <c r="AF1" t="inlineStr">
+      <c r="BJ1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i2840</t>
         </is>
       </c>
-      <c r="AG1" t="inlineStr">
+      <c r="BK1" t="inlineStr">
         <is>
           <t>prt_order_i2840</t>
         </is>
       </c>
-      <c r="AH1" t="inlineStr">
+      <c r="BL1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i3064</t>
         </is>
       </c>
-      <c r="AI1" t="inlineStr">
+      <c r="BM1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i3064</t>
         </is>
       </c>
-      <c r="AJ1" t="inlineStr">
+      <c r="BN1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i3064</t>
         </is>
       </c>
-      <c r="AK1" t="inlineStr">
+      <c r="BO1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i3064</t>
         </is>
       </c>
-      <c r="AL1" t="inlineStr">
+      <c r="BP1" t="inlineStr">
         <is>
           <t>prt_order_i3064</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
+      <c r="BQ1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i3350</t>
+        </is>
+      </c>
+      <c r="BR1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i3350</t>
+        </is>
+      </c>
+      <c r="BS1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i3350</t>
+        </is>
+      </c>
+      <c r="BT1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i3350</t>
+        </is>
+      </c>
+      <c r="BU1" t="inlineStr">
+        <is>
+          <t>prt_order_i3350</t>
+        </is>
+      </c>
+      <c r="BV1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i3500</t>
+        </is>
+      </c>
+      <c r="BW1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i3500</t>
+        </is>
+      </c>
+      <c r="BX1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i3500</t>
+        </is>
+      </c>
+      <c r="BY1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i3500</t>
+        </is>
+      </c>
+      <c r="BZ1" t="inlineStr">
+        <is>
+          <t>prt_order_i3500</t>
+        </is>
+      </c>
+      <c r="CA1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i5594</t>
         </is>
       </c>
-      <c r="AN1" t="inlineStr">
+      <c r="CB1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i5594</t>
         </is>
       </c>
-      <c r="AO1" t="inlineStr">
+      <c r="CC1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i5594</t>
         </is>
       </c>
-      <c r="AP1" t="inlineStr">
+      <c r="CD1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i5594</t>
         </is>
       </c>
-      <c r="AQ1" t="inlineStr">
+      <c r="CE1" t="inlineStr">
         <is>
           <t>prt_order_i5594</t>
         </is>
       </c>
-      <c r="AR1" t="inlineStr">
+      <c r="CF1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i6311</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
+      <c r="CG1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i6311</t>
         </is>
       </c>
-      <c r="AT1" t="inlineStr">
+      <c r="CH1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i6311</t>
         </is>
       </c>
-      <c r="AU1" t="inlineStr">
+      <c r="CI1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i6311</t>
         </is>
       </c>
-      <c r="AV1" t="inlineStr">
+      <c r="CJ1" t="inlineStr">
         <is>
           <t>prt_order_i6311</t>
         </is>
       </c>
-      <c r="AW1" t="inlineStr">
+      <c r="CK1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i7010</t>
         </is>
       </c>
-      <c r="AX1" t="inlineStr">
+      <c r="CL1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i7010</t>
         </is>
       </c>
-      <c r="AY1" t="inlineStr">
+      <c r="CM1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i7010</t>
         </is>
       </c>
-      <c r="AZ1" t="inlineStr">
+      <c r="CN1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i7010</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
+      <c r="CO1" t="inlineStr">
         <is>
           <t>prt_order_i7010</t>
         </is>
       </c>
-      <c r="BB1" t="inlineStr">
+      <c r="CP1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i7175</t>
         </is>
       </c>
-      <c r="BC1" t="inlineStr">
+      <c r="CQ1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i7175</t>
         </is>
       </c>
-      <c r="BD1" t="inlineStr">
+      <c r="CR1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i7175</t>
         </is>
       </c>
-      <c r="BE1" t="inlineStr">
+      <c r="CS1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i7175</t>
         </is>
       </c>
-      <c r="BF1" t="inlineStr">
+      <c r="CT1" t="inlineStr">
         <is>
           <t>prt_order_i7175</t>
         </is>
       </c>
-      <c r="BG1" t="inlineStr">
+      <c r="CU1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i7180</t>
+        </is>
+      </c>
+      <c r="CV1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i7180</t>
+        </is>
+      </c>
+      <c r="CW1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i7180</t>
+        </is>
+      </c>
+      <c r="CX1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i7180</t>
+        </is>
+      </c>
+      <c r="CY1" t="inlineStr">
+        <is>
+          <t>prt_order_i7180</t>
+        </is>
+      </c>
+      <c r="CZ1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.response_raw_i7513</t>
+        </is>
+      </c>
+      <c r="DA1" t="inlineStr">
+        <is>
+          <t>prt_1_vas.rt_raw_i7513</t>
+        </is>
+      </c>
+      <c r="DB1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.keys_raw_i7513</t>
+        </is>
+      </c>
+      <c r="DC1" t="inlineStr">
+        <is>
+          <t>prt_image_intens_resp.rt_raw_i7513</t>
+        </is>
+      </c>
+      <c r="DD1" t="inlineStr">
+        <is>
+          <t>prt_order_i7513</t>
+        </is>
+      </c>
+      <c r="DE1" t="inlineStr">
         <is>
           <t>prt_1_vas.response_raw_i8380</t>
         </is>
       </c>
-      <c r="BH1" t="inlineStr">
+      <c r="DF1" t="inlineStr">
         <is>
           <t>prt_1_vas.rt_raw_i8380</t>
         </is>
       </c>
-      <c r="BI1" t="inlineStr">
+      <c r="DG1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.keys_raw_i8380</t>
         </is>
       </c>
-      <c r="BJ1" t="inlineStr">
+      <c r="DH1" t="inlineStr">
         <is>
           <t>prt_image_intens_resp.rt_raw_i8380</t>
         </is>
       </c>
-      <c r="BK1" t="inlineStr">
+      <c r="DI1" t="inlineStr">
         <is>
           <t>prt_order_i8380</t>
         </is>
@@ -5543,6 +5793,2541 @@
       </c>
       <c r="BK26" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>779</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2019_May_06_1025</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>7.824491178076642</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>17.952</v>
+      </c>
+      <c r="K27" t="n">
+        <v>4</v>
+      </c>
+      <c r="L27" t="n">
+        <v>10.05988289516426</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="n">
+        <v>3.016</v>
+      </c>
+      <c r="P27" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>2.98733462555083</v>
+      </c>
+      <c r="R27" t="n">
+        <v>4</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
+        <v>1.297</v>
+      </c>
+      <c r="U27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V27" t="n">
+        <v>3.754359281145298</v>
+      </c>
+      <c r="W27" t="n">
+        <v>10</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>1.564</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>5.139140640281767</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>1.231</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>2.954233745146666</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>1.718</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>3.753896258227542</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>1.615</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>1.618790317322237</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" t="n">
+        <v>1.381</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>3.020682191105152</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>7</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX27" t="n">
+        <v>0.764</v>
+      </c>
+      <c r="AY27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>2.253075226351029</v>
+      </c>
+      <c r="BA27" t="n">
+        <v>8</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC27" t="n">
+        <v>1.465</v>
+      </c>
+      <c r="BD27" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE27" t="n">
+        <v>2.13550736765319</v>
+      </c>
+      <c r="BF27" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH27" t="n">
+        <v>2.098</v>
+      </c>
+      <c r="BI27" t="n">
+        <v>4</v>
+      </c>
+      <c r="BJ27" t="n">
+        <v>4.405286273458842</v>
+      </c>
+      <c r="BK27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>689</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2019_May_13_0917</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>15</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.505</v>
+      </c>
+      <c r="F28" t="n">
+        <v>3</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2.386319972645197</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3</v>
+      </c>
+      <c r="I28" t="n">
+        <v>12</v>
+      </c>
+      <c r="J28" t="n">
+        <v>2.988</v>
+      </c>
+      <c r="K28" t="n">
+        <v>6</v>
+      </c>
+      <c r="L28" t="n">
+        <v>1.58573543878515</v>
+      </c>
+      <c r="M28" t="n">
+        <v>10</v>
+      </c>
+      <c r="N28" t="n">
+        <v>-8</v>
+      </c>
+      <c r="O28" t="n">
+        <v>11.305</v>
+      </c>
+      <c r="P28" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>3.471066865938155</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="n">
+        <v>-10</v>
+      </c>
+      <c r="T28" t="n">
+        <v>3.423</v>
+      </c>
+      <c r="U28" t="n">
+        <v>6</v>
+      </c>
+      <c r="V28" t="n">
+        <v>2.419881843273743</v>
+      </c>
+      <c r="W28" t="n">
+        <v>6</v>
+      </c>
+      <c r="X28" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>2.803519522421311</v>
+      </c>
+      <c r="AB28" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC28" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>6.863</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>3.370637554753102</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>2.622</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>1.668935513782117</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>-12</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>4.757</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>2.519657332273255</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>-14</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>4.808</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU28" t="n">
+        <v>2.20304033325715</v>
+      </c>
+      <c r="AV28" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AX28" t="n">
+        <v>2.488</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ28" t="n">
+        <v>1.352042082591879</v>
+      </c>
+      <c r="BA28" t="n">
+        <v>11</v>
+      </c>
+      <c r="BB28" t="n">
+        <v>17</v>
+      </c>
+      <c r="BC28" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="BD28" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE28" t="n">
+        <v>2.736768063189857</v>
+      </c>
+      <c r="BF28" t="n">
+        <v>5</v>
+      </c>
+      <c r="BG28" t="n">
+        <v>19</v>
+      </c>
+      <c r="BH28" t="n">
+        <v>3.872</v>
+      </c>
+      <c r="BI28" t="n">
+        <v>7</v>
+      </c>
+      <c r="BJ28" t="n">
+        <v>1.96931723055809</v>
+      </c>
+      <c r="BK28" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>802</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2019_May_06_0922</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.413</v>
+      </c>
+      <c r="F29" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.502421330423203</v>
+      </c>
+      <c r="H29" t="n">
+        <v>7</v>
+      </c>
+      <c r="I29" t="n">
+        <v>8</v>
+      </c>
+      <c r="J29" t="n">
+        <v>3.138</v>
+      </c>
+      <c r="K29" t="n">
+        <v>7</v>
+      </c>
+      <c r="L29" t="n">
+        <v>2.80360166327705</v>
+      </c>
+      <c r="M29" t="n">
+        <v>9</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-20</v>
+      </c>
+      <c r="O29" t="n">
+        <v>16.545</v>
+      </c>
+      <c r="P29" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>4.505401082710478</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="n">
+        <v>-5</v>
+      </c>
+      <c r="T29" t="n">
+        <v>5.39</v>
+      </c>
+      <c r="U29" t="n">
+        <v>4</v>
+      </c>
+      <c r="V29" t="n">
+        <v>2.086328084037632</v>
+      </c>
+      <c r="W29" t="n">
+        <v>3</v>
+      </c>
+      <c r="X29" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>3.222</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>2.552505326566461</v>
+      </c>
+      <c r="AB29" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>3.858</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>1.235132111766006</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>1.234860187210415</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM29" t="n">
+        <v>-19</v>
+      </c>
+      <c r="AN29" t="n">
+        <v>7.508</v>
+      </c>
+      <c r="AO29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP29" t="n">
+        <v>3.721051377515778</v>
+      </c>
+      <c r="AQ29" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR29" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AS29" t="n">
+        <v>3.291</v>
+      </c>
+      <c r="AT29" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>2.803214959516481</v>
+      </c>
+      <c r="AV29" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX29" t="n">
+        <v>1.264</v>
+      </c>
+      <c r="AY29" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ29" t="n">
+        <v>2.669410350379849</v>
+      </c>
+      <c r="BA29" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC29" t="n">
+        <v>2.999</v>
+      </c>
+      <c r="BD29" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE29" t="n">
+        <v>1.869488532445757</v>
+      </c>
+      <c r="BF29" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG29" t="n">
+        <v>5</v>
+      </c>
+      <c r="BH29" t="n">
+        <v>3.339</v>
+      </c>
+      <c r="BI29" t="n">
+        <v>6</v>
+      </c>
+      <c r="BJ29" t="n">
+        <v>1.719097126343286</v>
+      </c>
+      <c r="BK29" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>717</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2019_May_06_1117</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1.829</v>
+      </c>
+      <c r="F30" t="n">
+        <v>5</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.718641014214882</v>
+      </c>
+      <c r="H30" t="n">
+        <v>9</v>
+      </c>
+      <c r="I30" t="n">
+        <v>10</v>
+      </c>
+      <c r="J30" t="n">
+        <v>7.814</v>
+      </c>
+      <c r="K30" t="n">
+        <v>7</v>
+      </c>
+      <c r="L30" t="n">
+        <v>2.452935868772329</v>
+      </c>
+      <c r="M30" t="n">
+        <v>6</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1.976</v>
+      </c>
+      <c r="P30" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>5.088928944760482</v>
+      </c>
+      <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0</v>
+      </c>
+      <c r="T30" t="n">
+        <v>17.363</v>
+      </c>
+      <c r="U30" t="n">
+        <v>6</v>
+      </c>
+      <c r="V30" t="n">
+        <v>5.78941982116703</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>-15</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>5.666</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>5.338711329999569</v>
+      </c>
+      <c r="AB30" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC30" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>5.977</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>1.652482520959893</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" t="n">
+        <v>1.782</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>2.653370407217153</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM30" t="n">
+        <v>-25</v>
+      </c>
+      <c r="AN30" t="n">
+        <v>6.997</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>3.003448784587817</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR30" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AS30" t="n">
+        <v>7.421</v>
+      </c>
+      <c r="AT30" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU30" t="n">
+        <v>3.120695141324177</v>
+      </c>
+      <c r="AV30" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX30" t="n">
+        <v>1.409</v>
+      </c>
+      <c r="AY30" t="n">
+        <v>7</v>
+      </c>
+      <c r="AZ30" t="n">
+        <v>1.485118816006434</v>
+      </c>
+      <c r="BA30" t="n">
+        <v>11</v>
+      </c>
+      <c r="BB30" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC30" t="n">
+        <v>4.994</v>
+      </c>
+      <c r="BD30" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE30" t="n">
+        <v>3.42041549471287</v>
+      </c>
+      <c r="BF30" t="n">
+        <v>8</v>
+      </c>
+      <c r="BG30" t="n">
+        <v>15</v>
+      </c>
+      <c r="BH30" t="n">
+        <v>15.877</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>7</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>4.004811712526134</v>
+      </c>
+      <c r="BK30" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>748</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2019_May_07_2013</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.271</v>
+      </c>
+      <c r="F31" t="n">
+        <v>6</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.652487027996813</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5</v>
+      </c>
+      <c r="I31" t="n">
+        <v>-10</v>
+      </c>
+      <c r="J31" t="n">
+        <v>10.887</v>
+      </c>
+      <c r="K31" t="n">
+        <v>6</v>
+      </c>
+      <c r="L31" t="n">
+        <v>6.924163696779942</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" t="n">
+        <v>-30</v>
+      </c>
+      <c r="O31" t="n">
+        <v>3.721</v>
+      </c>
+      <c r="P31" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>1.66951341128879</v>
+      </c>
+      <c r="R31" t="n">
+        <v>2</v>
+      </c>
+      <c r="S31" t="n">
+        <v>-20</v>
+      </c>
+      <c r="T31" t="n">
+        <v>2.483</v>
+      </c>
+      <c r="U31" t="n">
+        <v>7</v>
+      </c>
+      <c r="V31" t="n">
+        <v>3.070096742043461</v>
+      </c>
+      <c r="W31" t="n">
+        <v>4</v>
+      </c>
+      <c r="X31" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>5.799</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>4.238394905966288</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>5.015</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>1.284920145823889</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>2.856</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>2.970247547496001</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>-35</v>
+      </c>
+      <c r="AN31" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="AO31" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP31" t="n">
+        <v>2.35308006390369</v>
+      </c>
+      <c r="AQ31" t="n">
+        <v>7</v>
+      </c>
+      <c r="AR31" t="n">
+        <v>-20</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>5.889</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU31" t="n">
+        <v>4.755446378430861</v>
+      </c>
+      <c r="AV31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX31" t="n">
+        <v>9.244999999999999</v>
+      </c>
+      <c r="AY31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ31" t="n">
+        <v>1.935842631100058</v>
+      </c>
+      <c r="BA31" t="n">
+        <v>9</v>
+      </c>
+      <c r="BB31" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC31" t="n">
+        <v>4.592</v>
+      </c>
+      <c r="BD31" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE31" t="n">
+        <v>0.8180241811537599</v>
+      </c>
+      <c r="BF31" t="n">
+        <v>3</v>
+      </c>
+      <c r="BG31" t="n">
+        <v>10</v>
+      </c>
+      <c r="BH31" t="n">
+        <v>2.437</v>
+      </c>
+      <c r="BI31" t="n">
+        <v>7</v>
+      </c>
+      <c r="BJ31" t="n">
+        <v>3.387380116576423</v>
+      </c>
+      <c r="BK31" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>761</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2019_May_13_1115</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.183</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>4.538528635668627</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>5</v>
+      </c>
+      <c r="J32" t="n">
+        <v>5.323</v>
+      </c>
+      <c r="K32" t="n">
+        <v>6</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.619282886866131</v>
+      </c>
+      <c r="M32" t="n">
+        <v>10</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="n">
+        <v>12.128</v>
+      </c>
+      <c r="P32" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>5.355030554768746</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-5</v>
+      </c>
+      <c r="T32" t="n">
+        <v>6.22</v>
+      </c>
+      <c r="U32" t="n">
+        <v>6</v>
+      </c>
+      <c r="V32" t="n">
+        <v>5.054850453199833</v>
+      </c>
+      <c r="W32" t="n">
+        <v>9</v>
+      </c>
+      <c r="X32" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>6.339</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>2.670818858203347</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>3.671</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>2.57006834485037</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>3.291</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>2.235718522339084</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>7</v>
+      </c>
+      <c r="AM32" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AN32" t="n">
+        <v>6.603</v>
+      </c>
+      <c r="AO32" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP32" t="n">
+        <v>4.070612796043861</v>
+      </c>
+      <c r="AQ32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR32" t="n">
+        <v>-5</v>
+      </c>
+      <c r="AS32" t="n">
+        <v>5.557</v>
+      </c>
+      <c r="AT32" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU32" t="n">
+        <v>3.587754896005208</v>
+      </c>
+      <c r="AV32" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX32" t="n">
+        <v>5.792</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ32" t="n">
+        <v>2.335936903755282</v>
+      </c>
+      <c r="BA32" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC32" t="n">
+        <v>2.103</v>
+      </c>
+      <c r="BD32" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE32" t="n">
+        <v>2.586611007649481</v>
+      </c>
+      <c r="BF32" t="n">
+        <v>8</v>
+      </c>
+      <c r="BG32" t="n">
+        <v>5</v>
+      </c>
+      <c r="BH32" t="n">
+        <v>6.525</v>
+      </c>
+      <c r="BI32" t="n">
+        <v>6</v>
+      </c>
+      <c r="BJ32" t="n">
+        <v>3.170204998494228</v>
+      </c>
+      <c r="BK32" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>813</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2019_May_13_1021</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>25</v>
+      </c>
+      <c r="E33" t="n">
+        <v>7.681</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>4.788802814319752</v>
+      </c>
+      <c r="H33" t="n">
+        <v>4</v>
+      </c>
+      <c r="I33" t="n">
+        <v>30</v>
+      </c>
+      <c r="J33" t="n">
+        <v>4.563</v>
+      </c>
+      <c r="K33" t="n">
+        <v>5</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.622933894851485</v>
+      </c>
+      <c r="M33" t="n">
+        <v>3</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" t="n">
+        <v>11.305</v>
+      </c>
+      <c r="P33" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>4.555263298640966</v>
+      </c>
+      <c r="R33" t="n">
+        <v>5</v>
+      </c>
+      <c r="S33" t="n">
+        <v>-5</v>
+      </c>
+      <c r="T33" t="n">
+        <v>4.965</v>
+      </c>
+      <c r="U33" t="n">
+        <v>6</v>
+      </c>
+      <c r="V33" t="n">
+        <v>5.539187866309476</v>
+      </c>
+      <c r="W33" t="n">
+        <v>9</v>
+      </c>
+      <c r="X33" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>6.231</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>6.974234117619744</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>7.015</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>3.887360799873932</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>11.038</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>4.888973120577248</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>-15</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>9.265000000000001</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>3.737832927999989</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>-12</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>8.798</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>2.870133666974652</v>
+      </c>
+      <c r="AV33" t="n">
+        <v>6</v>
+      </c>
+      <c r="AW33" t="n">
+        <v>10</v>
+      </c>
+      <c r="AX33" t="n">
+        <v>4.763</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ33" t="n">
+        <v>4.471486021245255</v>
+      </c>
+      <c r="BA33" t="n">
+        <v>8</v>
+      </c>
+      <c r="BB33" t="n">
+        <v>5</v>
+      </c>
+      <c r="BC33" t="n">
+        <v>4.461</v>
+      </c>
+      <c r="BD33" t="n">
+        <v>4</v>
+      </c>
+      <c r="BE33" t="n">
+        <v>4.004837863515604</v>
+      </c>
+      <c r="BF33" t="n">
+        <v>11</v>
+      </c>
+      <c r="BG33" t="n">
+        <v>11</v>
+      </c>
+      <c r="BH33" t="n">
+        <v>12.975</v>
+      </c>
+      <c r="BI33" t="n">
+        <v>3</v>
+      </c>
+      <c r="BJ33" t="n">
+        <v>7.99217937323192</v>
+      </c>
+      <c r="BK33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>792</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2019_May_13_1217</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>15</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4.745</v>
+      </c>
+      <c r="F34" t="n">
+        <v>5</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2.152904250506253</v>
+      </c>
+      <c r="H34" t="n">
+        <v>11</v>
+      </c>
+      <c r="I34" t="n">
+        <v>15</v>
+      </c>
+      <c r="J34" t="n">
+        <v>24.605</v>
+      </c>
+      <c r="K34" t="n">
+        <v>5</v>
+      </c>
+      <c r="L34" t="n">
+        <v>4.321550411914359</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" t="n">
+        <v>10</v>
+      </c>
+      <c r="O34" t="n">
+        <v>16.174</v>
+      </c>
+      <c r="P34" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>4.454913611940356</v>
+      </c>
+      <c r="R34" t="n">
+        <v>5</v>
+      </c>
+      <c r="S34" t="n">
+        <v>16</v>
+      </c>
+      <c r="T34" t="n">
+        <v>19.043</v>
+      </c>
+      <c r="U34" t="n">
+        <v>6</v>
+      </c>
+      <c r="V34" t="n">
+        <v>10.81138041213671</v>
+      </c>
+      <c r="W34" t="n">
+        <v>1</v>
+      </c>
+      <c r="X34" t="n">
+        <v>12</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>5.88</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>2.703367845289904</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>9.369</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>3.570689716301786</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>10.634</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>4.438725503452588</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM34" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN34" t="n">
+        <v>6.797</v>
+      </c>
+      <c r="AO34" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP34" t="n">
+        <v>4.68854777559136</v>
+      </c>
+      <c r="AQ34" t="n">
+        <v>7</v>
+      </c>
+      <c r="AR34" t="n">
+        <v>15</v>
+      </c>
+      <c r="AS34" t="n">
+        <v>11.352</v>
+      </c>
+      <c r="AT34" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU34" t="n">
+        <v>12.71272567531923</v>
+      </c>
+      <c r="AV34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>19</v>
+      </c>
+      <c r="AX34" t="n">
+        <v>8.782999999999999</v>
+      </c>
+      <c r="AY34" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ34" t="n">
+        <v>2.102612524420692</v>
+      </c>
+      <c r="BA34" t="n">
+        <v>10</v>
+      </c>
+      <c r="BB34" t="n">
+        <v>15</v>
+      </c>
+      <c r="BC34" t="n">
+        <v>8.997999999999999</v>
+      </c>
+      <c r="BD34" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE34" t="n">
+        <v>4.171527365882866</v>
+      </c>
+      <c r="BF34" t="n">
+        <v>6</v>
+      </c>
+      <c r="BG34" t="n">
+        <v>20</v>
+      </c>
+      <c r="BH34" t="n">
+        <v>8.329000000000001</v>
+      </c>
+      <c r="BI34" t="n">
+        <v>6</v>
+      </c>
+      <c r="BJ34" t="n">
+        <v>4.68890082755388</v>
+      </c>
+      <c r="BK34" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>703</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2019_May_02_0937</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>30</v>
+      </c>
+      <c r="E35" t="n">
+        <v>6.357</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4.139047620192287</v>
+      </c>
+      <c r="H35" t="n">
+        <v>3</v>
+      </c>
+      <c r="I35" t="n">
+        <v>25</v>
+      </c>
+      <c r="J35" t="n">
+        <v>17.579</v>
+      </c>
+      <c r="K35" t="n">
+        <v>7</v>
+      </c>
+      <c r="L35" t="n">
+        <v>6.824188146722463</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0</v>
+      </c>
+      <c r="N35" t="n">
+        <v>-15</v>
+      </c>
+      <c r="O35" t="n">
+        <v>11.015</v>
+      </c>
+      <c r="P35" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>1.885733292549503</v>
+      </c>
+      <c r="R35" t="n">
+        <v>7</v>
+      </c>
+      <c r="S35" t="n">
+        <v>-32</v>
+      </c>
+      <c r="T35" t="n">
+        <v>7.845</v>
+      </c>
+      <c r="U35" t="n">
+        <v>8</v>
+      </c>
+      <c r="V35" t="n">
+        <v>3.704741346932224</v>
+      </c>
+      <c r="W35" t="n">
+        <v>10</v>
+      </c>
+      <c r="X35" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>8.929</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>3.587573006550883</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>3.841</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>2.052439120393956</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>7.861</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>3.771133665011803</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM35" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>13.05</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>4.855497057503271</v>
+      </c>
+      <c r="AQ35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR35" t="n">
+        <v>-25</v>
+      </c>
+      <c r="AS35" t="n">
+        <v>4.858</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU35" t="n">
+        <v>4.054995513992253</v>
+      </c>
+      <c r="AV35" t="n">
+        <v>8</v>
+      </c>
+      <c r="AW35" t="n">
+        <v>8</v>
+      </c>
+      <c r="AX35" t="n">
+        <v>6.159</v>
+      </c>
+      <c r="AY35" t="n">
+        <v>6</v>
+      </c>
+      <c r="AZ35" t="n">
+        <v>6.474517190755705</v>
+      </c>
+      <c r="BA35" t="n">
+        <v>6</v>
+      </c>
+      <c r="BB35" t="n">
+        <v>9</v>
+      </c>
+      <c r="BC35" t="n">
+        <v>5.143</v>
+      </c>
+      <c r="BD35" t="n">
+        <v>4</v>
+      </c>
+      <c r="BE35" t="n">
+        <v>3.637686794309957</v>
+      </c>
+      <c r="BF35" t="n">
+        <v>11</v>
+      </c>
+      <c r="BG35" t="n">
+        <v>20</v>
+      </c>
+      <c r="BH35" t="n">
+        <v>5.376</v>
+      </c>
+      <c r="BI35" t="n">
+        <v>6</v>
+      </c>
+      <c r="BJ35" t="n">
+        <v>3.754430571439116</v>
+      </c>
+      <c r="BK35" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>845</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>2019_May_02_1542</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2.546</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2.653289280553508</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7</v>
+      </c>
+      <c r="I36" t="n">
+        <v>20</v>
+      </c>
+      <c r="J36" t="n">
+        <v>6.077</v>
+      </c>
+      <c r="K36" t="n">
+        <v>2</v>
+      </c>
+      <c r="L36" t="n">
+        <v>3.58762355665931</v>
+      </c>
+      <c r="M36" t="n">
+        <v>9</v>
+      </c>
+      <c r="N36" t="n">
+        <v>3</v>
+      </c>
+      <c r="O36" t="n">
+        <v>5.293</v>
+      </c>
+      <c r="P36" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>3.654254988313369</v>
+      </c>
+      <c r="R36" t="n">
+        <v>3</v>
+      </c>
+      <c r="S36" t="n">
+        <v>0</v>
+      </c>
+      <c r="T36" t="n">
+        <v>10.955</v>
+      </c>
+      <c r="U36" t="n">
+        <v>6</v>
+      </c>
+      <c r="V36" t="n">
+        <v>7.608284414456193</v>
+      </c>
+      <c r="W36" t="n">
+        <v>0</v>
+      </c>
+      <c r="X36" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>4.059</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>6.256837400233053</v>
+      </c>
+      <c r="AB36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>3.058</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>1.20196963519129</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>2.392</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>1.418771027204457</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>11</v>
+      </c>
+      <c r="AM36" t="n">
+        <v>-20</v>
+      </c>
+      <c r="AN36" t="n">
+        <v>5.909</v>
+      </c>
+      <c r="AO36" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP36" t="n">
+        <v>3.404254162023335</v>
+      </c>
+      <c r="AQ36" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR36" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AS36" t="n">
+        <v>3.582</v>
+      </c>
+      <c r="AT36" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU36" t="n">
+        <v>1.40215598614077</v>
+      </c>
+      <c r="AV36" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX36" t="n">
+        <v>2.506</v>
+      </c>
+      <c r="AY36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ36" t="n">
+        <v>1.869678128461601</v>
+      </c>
+      <c r="BA36" t="n">
+        <v>6</v>
+      </c>
+      <c r="BB36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC36" t="n">
+        <v>3.28</v>
+      </c>
+      <c r="BD36" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE36" t="n">
+        <v>1.535697684795196</v>
+      </c>
+      <c r="BF36" t="n">
+        <v>8</v>
+      </c>
+      <c r="BG36" t="n">
+        <v>10</v>
+      </c>
+      <c r="BH36" t="n">
+        <v>4.877</v>
+      </c>
+      <c r="BI36" t="n">
+        <v>5</v>
+      </c>
+      <c r="BJ36" t="n">
+        <v>3.337620627085244</v>
+      </c>
+      <c r="BK36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>840</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2019_May_01_2029</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>31</v>
+      </c>
+      <c r="E37" t="n">
+        <v>7.359</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2.45299506119045</v>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" t="n">
+        <v>15</v>
+      </c>
+      <c r="J37" t="n">
+        <v>8.743</v>
+      </c>
+      <c r="K37" t="n">
+        <v>4</v>
+      </c>
+      <c r="L37" t="n">
+        <v>2.58679065625256</v>
+      </c>
+      <c r="M37" t="n">
+        <v>4</v>
+      </c>
+      <c r="N37" t="n">
+        <v>-21</v>
+      </c>
+      <c r="O37" t="n">
+        <v>4.706</v>
+      </c>
+      <c r="P37" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>2.019829459735774</v>
+      </c>
+      <c r="R37" t="n">
+        <v>5</v>
+      </c>
+      <c r="S37" t="n">
+        <v>-17</v>
+      </c>
+      <c r="T37" t="n">
+        <v>2.654</v>
+      </c>
+      <c r="U37" t="n">
+        <v>3</v>
+      </c>
+      <c r="V37" t="n">
+        <v>3.304115014772833</v>
+      </c>
+      <c r="W37" t="n">
+        <v>11</v>
+      </c>
+      <c r="X37" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>3.988</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>3.304219277559241</v>
+      </c>
+      <c r="AB37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC37" t="n">
+        <v>31</v>
+      </c>
+      <c r="AD37" t="n">
+        <v>20.43</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>4.372141825031576</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI37" t="n">
+        <v>5.524</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK37" t="n">
+        <v>2.25289794956916</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM37" t="n">
+        <v>-5</v>
+      </c>
+      <c r="AN37" t="n">
+        <v>6.574</v>
+      </c>
+      <c r="AO37" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP37" t="n">
+        <v>2.953597652014651</v>
+      </c>
+      <c r="AQ37" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR37" t="n">
+        <v>-20</v>
+      </c>
+      <c r="AS37" t="n">
+        <v>3.554</v>
+      </c>
+      <c r="AT37" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU37" t="n">
+        <v>2.05312834929282</v>
+      </c>
+      <c r="AV37" t="n">
+        <v>7</v>
+      </c>
+      <c r="AW37" t="n">
+        <v>6</v>
+      </c>
+      <c r="AX37" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="AY37" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ37" t="n">
+        <v>2.336764290086649</v>
+      </c>
+      <c r="BA37" t="n">
+        <v>8</v>
+      </c>
+      <c r="BB37" t="n">
+        <v>14</v>
+      </c>
+      <c r="BC37" t="n">
+        <v>1.853</v>
+      </c>
+      <c r="BD37" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE37" t="n">
+        <v>1.585988103224736</v>
+      </c>
+      <c r="BF37" t="n">
+        <v>10</v>
+      </c>
+      <c r="BG37" t="n">
+        <v>24</v>
+      </c>
+      <c r="BH37" t="n">
+        <v>2.453</v>
+      </c>
+      <c r="BI37" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ37" t="n">
+        <v>2.186905916207252</v>
+      </c>
+      <c r="BK37" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>787</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2019_May_01_1924</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>18</v>
+      </c>
+      <c r="E38" t="n">
+        <v>6.753</v>
+      </c>
+      <c r="F38" t="n">
+        <v>6</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2.536370134691424</v>
+      </c>
+      <c r="H38" t="n">
+        <v>8</v>
+      </c>
+      <c r="I38" t="n">
+        <v>39</v>
+      </c>
+      <c r="J38" t="n">
+        <v>4.275</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3</v>
+      </c>
+      <c r="L38" t="n">
+        <v>2.903526876511933</v>
+      </c>
+      <c r="M38" t="n">
+        <v>3</v>
+      </c>
+      <c r="N38" t="n">
+        <v>20</v>
+      </c>
+      <c r="O38" t="n">
+        <v>17.781</v>
+      </c>
+      <c r="P38" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>8.12502850700821</v>
+      </c>
+      <c r="R38" t="n">
+        <v>0</v>
+      </c>
+      <c r="S38" t="n">
+        <v>16</v>
+      </c>
+      <c r="T38" t="n">
+        <v>7.669</v>
+      </c>
+      <c r="U38" t="n">
+        <v>7</v>
+      </c>
+      <c r="V38" t="n">
+        <v>2.786565364503986</v>
+      </c>
+      <c r="W38" t="n">
+        <v>4</v>
+      </c>
+      <c r="X38" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>8.093999999999999</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>8.992744572099582</v>
+      </c>
+      <c r="AB38" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC38" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>7.242</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>2.136282277519967</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH38" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI38" t="n">
+        <v>8.519</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>2.219204544055174</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM38" t="n">
+        <v>-10</v>
+      </c>
+      <c r="AN38" t="n">
+        <v>7.425</v>
+      </c>
+      <c r="AO38" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP38" t="n">
+        <v>3.037329983303607</v>
+      </c>
+      <c r="AQ38" t="n">
+        <v>9</v>
+      </c>
+      <c r="AR38" t="n">
+        <v>16</v>
+      </c>
+      <c r="AS38" t="n">
+        <v>12.978</v>
+      </c>
+      <c r="AT38" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU38" t="n">
+        <v>4.754385421959341</v>
+      </c>
+      <c r="AV38" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW38" t="n">
+        <v>18</v>
+      </c>
+      <c r="AX38" t="n">
+        <v>6.708</v>
+      </c>
+      <c r="AY38" t="n">
+        <v>6</v>
+      </c>
+      <c r="AZ38" t="n">
+        <v>4.021494659612472</v>
+      </c>
+      <c r="BA38" t="n">
+        <v>7</v>
+      </c>
+      <c r="BB38" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC38" t="n">
+        <v>11.514</v>
+      </c>
+      <c r="BD38" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE38" t="n">
+        <v>3.737932333752724</v>
+      </c>
+      <c r="BF38" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG38" t="n">
+        <v>32</v>
+      </c>
+      <c r="BH38" t="n">
+        <v>8.544</v>
+      </c>
+      <c r="BI38" t="n">
+        <v>7</v>
+      </c>
+      <c r="BJ38" t="n">
+        <v>3.621182051537289</v>
+      </c>
+      <c r="BK38" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>812</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2019_May_06_1216</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>MAER M R1 P1 v1</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>-10</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.607</v>
+      </c>
+      <c r="F39" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1.669081937629016</v>
+      </c>
+      <c r="H39" t="n">
+        <v>8</v>
+      </c>
+      <c r="I39" t="n">
+        <v>15</v>
+      </c>
+      <c r="J39" t="n">
+        <v>4.859</v>
+      </c>
+      <c r="K39" t="n">
+        <v>8</v>
+      </c>
+      <c r="L39" t="n">
+        <v>0.9181383894665487</v>
+      </c>
+      <c r="M39" t="n">
+        <v>10</v>
+      </c>
+      <c r="N39" t="n">
+        <v>-40</v>
+      </c>
+      <c r="O39" t="n">
+        <v>8.872</v>
+      </c>
+      <c r="P39" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>4.137398820777889</v>
+      </c>
+      <c r="R39" t="n">
+        <v>4</v>
+      </c>
+      <c r="S39" t="n">
+        <v>-20</v>
+      </c>
+      <c r="T39" t="n">
+        <v>27.395</v>
+      </c>
+      <c r="U39" t="n">
+        <v>7</v>
+      </c>
+      <c r="V39" t="n">
+        <v>7.490679598055067</v>
+      </c>
+      <c r="W39" t="n">
+        <v>0</v>
+      </c>
+      <c r="X39" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>4.956</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>1.335135446974164</v>
+      </c>
+      <c r="AB39" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC39" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>6.024</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>6</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>4.421801258306004</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI39" t="n">
+        <v>6.876</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>4.071200665599463</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM39" t="n">
+        <v>-50</v>
+      </c>
+      <c r="AN39" t="n">
+        <v>4.975</v>
+      </c>
+      <c r="AO39" t="n">
+        <v>9</v>
+      </c>
+      <c r="AP39" t="n">
+        <v>3.470772917757131</v>
+      </c>
+      <c r="AQ39" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR39" t="n">
+        <v>-25</v>
+      </c>
+      <c r="AS39" t="n">
+        <v>4.607</v>
+      </c>
+      <c r="AT39" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU39" t="n">
+        <v>1.752441386735882</v>
+      </c>
+      <c r="AV39" t="n">
+        <v>9</v>
+      </c>
+      <c r="AW39" t="n">
+        <v>25</v>
+      </c>
+      <c r="AX39" t="n">
+        <v>6.128</v>
+      </c>
+      <c r="AY39" t="n">
+        <v>7</v>
+      </c>
+      <c r="AZ39" t="n">
+        <v>2.003285930322818</v>
+      </c>
+      <c r="BA39" t="n">
+        <v>6</v>
+      </c>
+      <c r="BB39" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC39" t="n">
+        <v>8.640000000000001</v>
+      </c>
+      <c r="BD39" t="n">
+        <v>5</v>
+      </c>
+      <c r="BE39" t="n">
+        <v>5.789130469402153</v>
+      </c>
+      <c r="BF39" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG39" t="n">
+        <v>40</v>
+      </c>
+      <c r="BH39" t="n">
+        <v>3.873</v>
+      </c>
+      <c r="BI39" t="n">
+        <v>8</v>
+      </c>
+      <c r="BJ39" t="n">
+        <v>4.087630617683317</v>
+      </c>
+      <c r="BK39" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>